<commit_message>
Font size fix on XLS files
</commit_message>
<xml_diff>
--- a/CHECON.ECO.xlsx
+++ b/CHECON.ECO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -52,7 +52,7 @@
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="M/D/YYYY"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <name val="Verdana"/>
@@ -75,14 +75,20 @@
       <family val="0"/>
     </font>
     <font>
+      <sz val="10"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <b val="true"/>
-      <sz val="11"/>
+      <sz val="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -144,28 +150,32 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -189,10 +199,10 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="1" width="14"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="1" width="10.2518518518519"/>
@@ -200,63 +210,63 @@
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="8.0037037037037"/>
     <col collapsed="false" hidden="false" max="249" min="6" style="1" width="13"/>
     <col collapsed="false" hidden="false" max="1017" min="250" style="2" width="13"/>
-    <col collapsed="false" hidden="false" max="1025" min="1018" style="0" width="13"/>
+    <col collapsed="false" hidden="false" max="1025" min="1018" style="3" width="13"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="5" t="n">
+      <c r="E2" s="6" t="n">
         <v>42206</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="5"/>
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="6"/>
     </row>
     <row r="4" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="5"/>
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="6"/>
     </row>
     <row r="5" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="5"/>
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="6"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>